<commit_message>
Added in addModuleDialog feature to select total of ects points (Bachelor 180 / Master 120)
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\Desktop\workspace\java_workspace\CurriculumRechner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E207CBB-2F41-4B32-A498-E6493766B21F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30088BC0-3EDF-43AC-931E-9CA4DBD6D07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>STEOP</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Kurs 1</t>
+  </si>
+  <si>
+    <t>Semester</t>
   </si>
 </sst>
 </file>
@@ -381,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -393,7 +396,7 @@
     <col min="2" max="2" width="7.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -406,8 +409,11 @@
       <c r="D1" t="s">
         <v>10</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -420,8 +426,11 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -434,8 +443,11 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -448,8 +460,11 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -462,8 +477,11 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -475,6 +493,9 @@
       </c>
       <c r="D6" t="s">
         <v>6</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added semester to Course Class
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\Desktop\workspace\java_workspace\CurriculumRechner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30088BC0-3EDF-43AC-931E-9CA4DBD6D07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3882AC-DA07-4A55-8EC1-33CBF6F9D65B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -407,10 +407,10 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -423,10 +423,10 @@
       <c r="C2">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -440,10 +440,10 @@
       <c r="C3">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -457,10 +457,10 @@
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -474,11 +474,11 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -491,11 +491,11 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete and edit added in semesterView
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\Desktop\workspace\java_workspace\CurriculumRechner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3882AC-DA07-4A55-8EC1-33CBF6F9D65B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6062EE91-03A0-4A31-B358-66E2B6C6B57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -441,7 +441,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>

</xml_diff>